<commit_message>
LOOP remove illegals and recode negatives
</commit_message>
<xml_diff>
--- a/Documentation/data/NLSY97_Religiosity_20042014.xlsx
+++ b/Documentation/data/NLSY97_Religiosity_20042014.xlsx
@@ -9,15 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="6165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="6165" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Layout" sheetId="1" r:id="rId1"/>
-    <sheet name="Renaming" sheetId="5" r:id="rId2"/>
+    <sheet name="Data Layout (2)" sheetId="6" r:id="rId1"/>
+    <sheet name="Data Layout" sheetId="1" r:id="rId2"/>
+    <sheet name="Renaming" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Renaming!$A$1:$F$134</definedName>
-    <definedName name="dsSourceLabels" localSheetId="1">Renaming!$A$2:$C$134</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Renaming!$A$1:$F$134</definedName>
+    <definedName name="dsSourceLabels" localSheetId="2">Renaming!$A$2:$C$134</definedName>
+    <definedName name="q">'Data Layout (2)'!$T$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="351">
   <si>
     <t>x</t>
   </si>
@@ -1739,6 +1742,9 @@
   </si>
   <si>
     <t>TI</t>
+  </si>
+  <si>
+    <t>RNUM</t>
   </si>
 </sst>
 </file>
@@ -2001,7 +2007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2145,12 +2151,14 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="5">
     <dxf>
       <fill>
         <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
@@ -2190,284 +2198,32 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.49803155613879818"/>
+          </stop>
+        </gradientFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2489,7 +2245,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1">
-      <tableStyleElement type="firstRowStripe" dxfId="31"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2770,10 +2526,1631 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X59"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="75.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="11.5703125" style="4" customWidth="1"/>
+    <col min="4" max="18" width="5.28515625" style="2" customWidth="1"/>
+    <col min="21" max="23" width="9.140625" style="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="25">
+        <v>1997</v>
+      </c>
+      <c r="E1" s="25">
+        <v>1998</v>
+      </c>
+      <c r="F1" s="25">
+        <v>1999</v>
+      </c>
+      <c r="G1" s="25">
+        <v>2000</v>
+      </c>
+      <c r="H1" s="25">
+        <v>2001</v>
+      </c>
+      <c r="I1" s="25">
+        <v>2002</v>
+      </c>
+      <c r="J1" s="25">
+        <v>2003</v>
+      </c>
+      <c r="K1" s="25">
+        <v>2004</v>
+      </c>
+      <c r="L1" s="25">
+        <v>2005</v>
+      </c>
+      <c r="M1" s="25">
+        <v>2006</v>
+      </c>
+      <c r="N1" s="25">
+        <v>2007</v>
+      </c>
+      <c r="O1" s="25">
+        <v>2008</v>
+      </c>
+      <c r="P1" s="25">
+        <v>2009</v>
+      </c>
+      <c r="Q1" s="25">
+        <v>2010</v>
+      </c>
+      <c r="R1" s="25">
+        <v>2011</v>
+      </c>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="X1" s="1"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="1" t="str">
+        <f>CONCATENATE(q,C2,q,)</f>
+        <v>"sample"</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X2" s="1"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1" t="str">
+        <f>CONCATENATE(q,C3,q,)</f>
+        <v>"id"</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1" t="str">
+        <f>CONCATENATE(q,C4,q,)</f>
+        <v>"sex"</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X4" s="1"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1" t="str">
+        <f>CONCATENATE(q,C5,q,)</f>
+        <v>"race"</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X5" s="1"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1" t="str">
+        <f>CONCATENATE(q,C6,q,)</f>
+        <v>"bmonth"</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X6" s="1"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1" t="str">
+        <f>CONCATENATE(q,C7,q,)</f>
+        <v>"byear"</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X7" s="1"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
+        <v>345</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1" t="str">
+        <f>CONCATENATE(q,C8,q,)</f>
+        <v>"attendPR"</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X8" s="1"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="46" t="s">
+        <v>346</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>342</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1" t="str">
+        <f>CONCATENATE(q,C9,q,)</f>
+        <v>"relprefPR"</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X9" s="1"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="46" t="s">
+        <v>347</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="52"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1" t="str">
+        <f>CONCATENATE(q,C10,q,)</f>
+        <v>"relraisedPR"</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X10" s="1"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1" t="str">
+        <f>CONCATENATE(q,C11,q,)</f>
+        <v>"agemon"</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X11" s="1"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1" t="str">
+        <f>CONCATENATE(q,C12,q,)</f>
+        <v>"ageyear"</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X12" s="1"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1" t="str">
+        <f>CONCATENATE(q,C13,q,)</f>
+        <v>"famrel"</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X13" s="1"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1" t="str">
+        <f>CONCATENATE(q,C14,q,)</f>
+        <v>"attend"</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X14" s="1"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1" t="str">
+        <f>CONCATENATE(q,C15,q,)</f>
+        <v>"values"</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X15" s="1"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1" t="str">
+        <f>CONCATENATE(q,C16,q,)</f>
+        <v>"todo"</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X16" s="1"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1" t="str">
+        <f>CONCATENATE(q,C17,q,)</f>
+        <v>"obeyed"</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X17" s="1"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1" t="str">
+        <f>CONCATENATE(q,C18,q,)</f>
+        <v>"pray"</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X18" s="1"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1" t="str">
+        <f>CONCATENATE(q,C19,q,)</f>
+        <v>"decisions"</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X19" s="1"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1" t="str">
+        <f>CONCATENATE(q,C20,q,)</f>
+        <v>"relpref"</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1" t="str">
+        <f>CONCATENATE(q,C21,q,)</f>
+        <v>"bornagain"</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X21" s="1"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="46" t="s">
+        <v>348</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>269</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1" t="str">
+        <f>CONCATENATE(q,C22,q,)</f>
+        <v>"faith"</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X22" s="1"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="33"/>
+      <c r="I23" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="33"/>
+      <c r="K23" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L23" s="33"/>
+      <c r="M23" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="R23" s="34"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1" t="str">
+        <f>CONCATENATE(q,C23,q,)</f>
+        <v>"calm"</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X23" s="1"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="14"/>
+      <c r="I24" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="14"/>
+      <c r="K24" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="14"/>
+      <c r="M24" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R24" s="15"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1" t="str">
+        <f>CONCATENATE(q,C24,q,)</f>
+        <v>"blue"</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="14"/>
+      <c r="I25" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="14"/>
+      <c r="K25" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="14"/>
+      <c r="M25" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R25" s="15"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1" t="str">
+        <f>CONCATENATE(q,C25,q,)</f>
+        <v>"happy"</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X25" s="1"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="14"/>
+      <c r="I26" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="14"/>
+      <c r="K26" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="14"/>
+      <c r="M26" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R26" s="15"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1" t="str">
+        <f>CONCATENATE(q,C26,q,)</f>
+        <v>"depressed"</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X26" s="1"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="18"/>
+      <c r="I27" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="18"/>
+      <c r="K27" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="18"/>
+      <c r="M27" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="R27" s="19"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1" t="str">
+        <f>CONCATENATE(q,C27,q,)</f>
+        <v>"nervous"</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X27" s="1"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="16"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P28" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R28" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1" t="str">
+        <f>CONCATENATE(q,C28,q,)</f>
+        <v>"tv"</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X28" s="1"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O29" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P29" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R29" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1" t="str">
+        <f>CONCATENATE(q,C29,q,)</f>
+        <v>"computer"</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X29" s="1"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="K30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="L30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="M30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="O30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="P30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="R30" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1" t="str">
+        <f>CONCATENATE(q,C30,q,)</f>
+        <v>"internet"</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="X30" s="1"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <v>1997</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1999</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2000</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2001</v>
+      </c>
+      <c r="I31" s="2">
+        <v>2002</v>
+      </c>
+      <c r="J31" s="2">
+        <v>2003</v>
+      </c>
+      <c r="K31" s="2">
+        <v>2004</v>
+      </c>
+      <c r="L31" s="2">
+        <v>2005</v>
+      </c>
+      <c r="M31" s="2">
+        <v>2006</v>
+      </c>
+      <c r="N31" s="2">
+        <v>2007</v>
+      </c>
+      <c r="O31" s="2">
+        <v>2008</v>
+      </c>
+      <c r="P31" s="2">
+        <v>2009</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>2010</v>
+      </c>
+      <c r="R31" s="2">
+        <v>2011</v>
+      </c>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="X31" s="1"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="X32" s="1"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="X33" s="1"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="I34" s="6"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="X34" s="1"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="X35" s="1"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="X36" s="1"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="X37" s="1"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="X38" s="1"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="X39" s="1"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="I40" s="6"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="X40" s="1"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="I41" s="6"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="X41" s="1"/>
+    </row>
+    <row r="43" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="M43" s="6"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="X43" s="1"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="M47" s="6"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="X47" s="1"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="M48" s="6"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="X48" s="1"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="M49" s="6"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="X49" s="1"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="M50" s="6"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="X50" s="1"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="M51" s="6"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="X51" s="1"/>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="M52" s="6"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="X52" s="1"/>
+    </row>
+    <row r="54" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="N54" s="6"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="X54" s="1"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="N55" s="6"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="X55" s="1"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="N56" s="6"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="X56" s="1"/>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="N57" s="6"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="X57" s="1"/>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="X58" s="1"/>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="X59" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D54:R57 D34:R34 D43:R43 B11:C12 B14:C14 D40:R41 N47:R51 D47:L51 M47:M52">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",B11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:R30">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.nlsinfo.org/investigator/pages/search.jsp"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3861,7 +5238,7 @@
       <c r="T27" s="1"/>
       <c r="X27" s="1"/>
     </row>
-    <row r="28" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>49</v>
       </c>
@@ -4190,7 +5567,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D53:R56 M42:M51 D33:R33 D42:L50 N42:R50 B8:C9 B11:C11 D37:R40">
-    <cfRule type="containsText" dxfId="30" priority="70" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="1" priority="70" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4208,12 +5585,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O134"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="F134" sqref="F133:F134"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4253,14 +5630,14 @@
         <v>63</v>
       </c>
       <c r="D2" t="str">
-        <f>RIGHT(C2,4)</f>
+        <f t="shared" ref="D2:D33" si="0">RIGHT(C2,4)</f>
         <v>1997</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>262</v>
       </c>
       <c r="F2" t="str">
-        <f>CONCATENATE($N$2,B2,$N$2,"=",$N$2,E2,"_",D2,$N$2,$O$2)</f>
+        <f t="shared" ref="F2:F44" si="1">CONCATENATE($N$2,B2,$N$2,"=",$N$2,E2,"_",D2,$N$2,$O$2)</f>
         <v>"R0323900"="famrel_1997",</v>
       </c>
       <c r="N2" t="s">
@@ -4281,14 +5658,14 @@
         <v>64</v>
       </c>
       <c r="D3" t="str">
-        <f>RIGHT(C3,4)</f>
+        <f t="shared" si="0"/>
         <v>1998</v>
       </c>
       <c r="E3" s="50" t="s">
         <v>262</v>
       </c>
       <c r="F3" t="str">
-        <f>CONCATENATE($N$2,B3,$N$2,"=",$N$2,E3,"_",D3,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R2165200"="famrel_1998",</v>
       </c>
     </row>
@@ -4303,14 +5680,14 @@
         <v>65</v>
       </c>
       <c r="D4" t="str">
-        <f>RIGHT(C4,4)</f>
+        <f t="shared" si="0"/>
         <v>1999</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>262</v>
       </c>
       <c r="F4" t="str">
-        <f>CONCATENATE($N$2,B4,$N$2,"=",$N$2,E4,"_",D4,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R3483100"="famrel_1999",</v>
       </c>
     </row>
@@ -4325,14 +5702,14 @@
         <v>66</v>
       </c>
       <c r="D5" t="str">
-        <f>RIGHT(C5,4)</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>262</v>
       </c>
       <c r="F5" t="str">
-        <f>CONCATENATE($N$2,B5,$N$2,"=",$N$2,E5,"_",D5,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R4881300"="famrel_2000",</v>
       </c>
     </row>
@@ -4347,14 +5724,14 @@
         <v>128</v>
       </c>
       <c r="D6" t="str">
-        <f>RIGHT(C6,4)</f>
+        <f t="shared" si="0"/>
         <v>2003</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F6" t="str">
-        <f>CONCATENATE($N$2,B6,$N$2,"=",$N$2,E6,"_",D6,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S2977900"="internet_2003",</v>
       </c>
     </row>
@@ -4369,14 +5746,14 @@
         <v>131</v>
       </c>
       <c r="D7" t="str">
-        <f>RIGHT(C7,4)</f>
+        <f t="shared" si="0"/>
         <v>2004</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F7" t="str">
-        <f>CONCATENATE($N$2,B7,$N$2,"=",$N$2,E7,"_",D7,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S4676700"="internet_2004",</v>
       </c>
     </row>
@@ -4391,14 +5768,14 @@
         <v>142</v>
       </c>
       <c r="D8" t="str">
-        <f>RIGHT(C8,4)</f>
+        <f t="shared" si="0"/>
         <v>2005</v>
       </c>
       <c r="E8" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F8" t="str">
-        <f>CONCATENATE($N$2,B8,$N$2,"=",$N$2,E8,"_",D8,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S6308900"="internet_2005",</v>
       </c>
     </row>
@@ -4413,14 +5790,14 @@
         <v>156</v>
       </c>
       <c r="D9" t="str">
-        <f>RIGHT(C9,4)</f>
+        <f t="shared" si="0"/>
         <v>2006</v>
       </c>
       <c r="E9" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F9" t="str">
-        <f>CONCATENATE($N$2,B9,$N$2,"=",$N$2,E9,"_",D9,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S8329800"="internet_2006",</v>
       </c>
     </row>
@@ -4435,14 +5812,14 @@
         <v>170</v>
       </c>
       <c r="D10" t="str">
-        <f>RIGHT(C10,4)</f>
+        <f t="shared" si="0"/>
         <v>2007</v>
       </c>
       <c r="E10" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F10" t="str">
-        <f>CONCATENATE($N$2,B10,$N$2,"=",$N$2,E10,"_",D10,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T0737600"="internet_2007",</v>
       </c>
     </row>
@@ -4457,14 +5834,14 @@
         <v>182</v>
       </c>
       <c r="D11" t="str">
-        <f>RIGHT(C11,4)</f>
+        <f t="shared" si="0"/>
         <v>2008</v>
       </c>
       <c r="E11" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F11" t="str">
-        <f>CONCATENATE($N$2,B11,$N$2,"=",$N$2,E11,"_",D11,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T2779700"="internet_2008",</v>
       </c>
     </row>
@@ -4479,14 +5856,14 @@
         <v>212</v>
       </c>
       <c r="D12" t="str">
-        <f>RIGHT(C12,4)</f>
+        <f t="shared" si="0"/>
         <v>2009</v>
       </c>
       <c r="E12" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F12" t="str">
-        <f>CONCATENATE($N$2,B12,$N$2,"=",$N$2,E12,"_",D12,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T4494400"="internet_2009",</v>
       </c>
     </row>
@@ -4501,14 +5878,14 @@
         <v>220</v>
       </c>
       <c r="D13" t="str">
-        <f>RIGHT(C13,4)</f>
+        <f t="shared" si="0"/>
         <v>2010</v>
       </c>
       <c r="E13" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F13" t="str">
-        <f>CONCATENATE($N$2,B13,$N$2,"=",$N$2,E13,"_",D13,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T6141400"="internet_2010",</v>
       </c>
     </row>
@@ -4523,14 +5900,14 @@
         <v>242</v>
       </c>
       <c r="D14" t="str">
-        <f>RIGHT(C14,4)</f>
+        <f t="shared" si="0"/>
         <v>2011</v>
       </c>
       <c r="E14" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F14" t="str">
-        <f>CONCATENATE($N$2,B14,$N$2,"=",$N$2,E14,"_",D14,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T7635300"="internet_2011",</v>
       </c>
     </row>
@@ -4545,14 +5922,14 @@
         <v>278</v>
       </c>
       <c r="D15" t="str">
-        <f>RIGHT(C15,4)</f>
+        <f t="shared" si="0"/>
         <v>1997</v>
       </c>
       <c r="E15" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F15" t="str">
-        <f>CONCATENATE($N$2,B15,$N$2,"=",$N$2,E15,"_",D15,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R1193900"="agemon_1997",</v>
       </c>
     </row>
@@ -4567,14 +5944,14 @@
         <v>282</v>
       </c>
       <c r="D16" t="str">
-        <f>RIGHT(C16,4)</f>
+        <f t="shared" si="0"/>
         <v>1998</v>
       </c>
       <c r="E16" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F16" t="str">
-        <f>CONCATENATE($N$2,B16,$N$2,"=",$N$2,E16,"_",D16,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R2553400"="agemon_1998",</v>
       </c>
     </row>
@@ -4589,14 +5966,14 @@
         <v>286</v>
       </c>
       <c r="D17" t="str">
-        <f>RIGHT(C17,4)</f>
+        <f t="shared" si="0"/>
         <v>1999</v>
       </c>
       <c r="E17" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F17" t="str">
-        <f>CONCATENATE($N$2,B17,$N$2,"=",$N$2,E17,"_",D17,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R3876200"="agemon_1999",</v>
       </c>
     </row>
@@ -4611,14 +5988,14 @@
         <v>290</v>
       </c>
       <c r="D18" t="str">
-        <f>RIGHT(C18,4)</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="E18" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F18" t="str">
-        <f>CONCATENATE($N$2,B18,$N$2,"=",$N$2,E18,"_",D18,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R5453600"="agemon_2000",</v>
       </c>
     </row>
@@ -4633,14 +6010,14 @@
         <v>294</v>
       </c>
       <c r="D19" t="str">
-        <f>RIGHT(C19,4)</f>
+        <f t="shared" si="0"/>
         <v>2001</v>
       </c>
       <c r="E19" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F19" t="str">
-        <f>CONCATENATE($N$2,B19,$N$2,"=",$N$2,E19,"_",D19,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R7215900"="agemon_2001",</v>
       </c>
     </row>
@@ -4655,14 +6032,14 @@
         <v>298</v>
       </c>
       <c r="D20" t="str">
-        <f>RIGHT(C20,4)</f>
+        <f t="shared" si="0"/>
         <v>2002</v>
       </c>
       <c r="E20" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F20" t="str">
-        <f>CONCATENATE($N$2,B20,$N$2,"=",$N$2,E20,"_",D20,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S1531300"="agemon_2002",</v>
       </c>
     </row>
@@ -4677,14 +6054,14 @@
         <v>302</v>
       </c>
       <c r="D21" t="str">
-        <f>RIGHT(C21,4)</f>
+        <f t="shared" si="0"/>
         <v>2003</v>
       </c>
       <c r="E21" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F21" t="str">
-        <f>CONCATENATE($N$2,B21,$N$2,"=",$N$2,E21,"_",D21,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S2000900"="agemon_2003",</v>
       </c>
     </row>
@@ -4699,14 +6076,14 @@
         <v>306</v>
       </c>
       <c r="D22" t="str">
-        <f>RIGHT(C22,4)</f>
+        <f t="shared" si="0"/>
         <v>2004</v>
       </c>
       <c r="E22" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F22" t="str">
-        <f>CONCATENATE($N$2,B22,$N$2,"=",$N$2,E22,"_",D22,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S3801000"="agemon_2004",</v>
       </c>
     </row>
@@ -4721,14 +6098,14 @@
         <v>310</v>
       </c>
       <c r="D23" t="str">
-        <f>RIGHT(C23,4)</f>
+        <f t="shared" si="0"/>
         <v>2005</v>
       </c>
       <c r="E23" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F23" t="str">
-        <f>CONCATENATE($N$2,B23,$N$2,"=",$N$2,E23,"_",D23,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S5400900"="agemon_2005",</v>
       </c>
     </row>
@@ -4743,14 +6120,14 @@
         <v>314</v>
       </c>
       <c r="D24" t="str">
-        <f>RIGHT(C24,4)</f>
+        <f t="shared" si="0"/>
         <v>2006</v>
       </c>
       <c r="E24" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F24" t="str">
-        <f>CONCATENATE($N$2,B24,$N$2,"=",$N$2,E24,"_",D24,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S7501100"="agemon_2006",</v>
       </c>
     </row>
@@ -4765,14 +6142,14 @@
         <v>318</v>
       </c>
       <c r="D25" t="str">
-        <f>RIGHT(C25,4)</f>
+        <f t="shared" si="0"/>
         <v>2007</v>
       </c>
       <c r="E25" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F25" t="str">
-        <f>CONCATENATE($N$2,B25,$N$2,"=",$N$2,E25,"_",D25,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T0008400"="agemon_2007",</v>
       </c>
     </row>
@@ -4787,14 +6164,14 @@
         <v>322</v>
       </c>
       <c r="D26" t="str">
-        <f>RIGHT(C26,4)</f>
+        <f t="shared" si="0"/>
         <v>2008</v>
       </c>
       <c r="E26" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F26" t="str">
-        <f>CONCATENATE($N$2,B26,$N$2,"=",$N$2,E26,"_",D26,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T2011000"="agemon_2008",</v>
       </c>
     </row>
@@ -4809,14 +6186,14 @@
         <v>326</v>
       </c>
       <c r="D27" t="str">
-        <f>RIGHT(C27,4)</f>
+        <f t="shared" si="0"/>
         <v>2009</v>
       </c>
       <c r="E27" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F27" t="str">
-        <f>CONCATENATE($N$2,B27,$N$2,"=",$N$2,E27,"_",D27,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T3601400"="agemon_2009",</v>
       </c>
     </row>
@@ -4831,14 +6208,14 @@
         <v>330</v>
       </c>
       <c r="D28" t="str">
-        <f>RIGHT(C28,4)</f>
+        <f t="shared" si="0"/>
         <v>2010</v>
       </c>
       <c r="E28" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F28" t="str">
-        <f>CONCATENATE($N$2,B28,$N$2,"=",$N$2,E28,"_",D28,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T5201300"="agemon_2010",</v>
       </c>
     </row>
@@ -4853,14 +6230,14 @@
         <v>334</v>
       </c>
       <c r="D29" t="str">
-        <f>RIGHT(C29,4)</f>
+        <f t="shared" si="0"/>
         <v>2011</v>
       </c>
       <c r="E29" s="50" t="s">
         <v>24</v>
       </c>
       <c r="F29" t="str">
-        <f>CONCATENATE($N$2,B29,$N$2,"=",$N$2,E29,"_",D29,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T6651200"="agemon_2011",</v>
       </c>
     </row>
@@ -4875,14 +6252,14 @@
         <v>280</v>
       </c>
       <c r="D30" t="str">
-        <f>RIGHT(C30,4)</f>
+        <f t="shared" si="0"/>
         <v>1997</v>
       </c>
       <c r="E30" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F30" t="str">
-        <f>CONCATENATE($N$2,B30,$N$2,"=",$N$2,E30,"_",D30,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R1194100"="ageyear_1997",</v>
       </c>
     </row>
@@ -4897,14 +6274,14 @@
         <v>284</v>
       </c>
       <c r="D31" t="str">
-        <f>RIGHT(C31,4)</f>
+        <f t="shared" si="0"/>
         <v>1998</v>
       </c>
       <c r="E31" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F31" t="str">
-        <f>CONCATENATE($N$2,B31,$N$2,"=",$N$2,E31,"_",D31,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R2553500"="ageyear_1998",</v>
       </c>
     </row>
@@ -4919,14 +6296,14 @@
         <v>288</v>
       </c>
       <c r="D32" t="str">
-        <f>RIGHT(C32,4)</f>
+        <f t="shared" si="0"/>
         <v>1999</v>
       </c>
       <c r="E32" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F32" t="str">
-        <f>CONCATENATE($N$2,B32,$N$2,"=",$N$2,E32,"_",D32,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R3876300"="ageyear_1999",</v>
       </c>
     </row>
@@ -4941,14 +6318,14 @@
         <v>292</v>
       </c>
       <c r="D33" t="str">
-        <f>RIGHT(C33,4)</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="E33" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F33" t="str">
-        <f>CONCATENATE($N$2,B33,$N$2,"=",$N$2,E33,"_",D33,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R5453700"="ageyear_2000",</v>
       </c>
     </row>
@@ -4963,14 +6340,14 @@
         <v>296</v>
       </c>
       <c r="D34" t="str">
-        <f>RIGHT(C34,4)</f>
+        <f t="shared" ref="D34:D65" si="2">RIGHT(C34,4)</f>
         <v>2001</v>
       </c>
       <c r="E34" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F34" t="str">
-        <f>CONCATENATE($N$2,B34,$N$2,"=",$N$2,E34,"_",D34,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"R7216000"="ageyear_2001",</v>
       </c>
     </row>
@@ -4985,14 +6362,14 @@
         <v>300</v>
       </c>
       <c r="D35" t="str">
-        <f>RIGHT(C35,4)</f>
+        <f t="shared" si="2"/>
         <v>2002</v>
       </c>
       <c r="E35" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F35" t="str">
-        <f>CONCATENATE($N$2,B35,$N$2,"=",$N$2,E35,"_",D35,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S1531400"="ageyear_2002",</v>
       </c>
     </row>
@@ -5007,14 +6384,14 @@
         <v>304</v>
       </c>
       <c r="D36" t="str">
-        <f>RIGHT(C36,4)</f>
+        <f t="shared" si="2"/>
         <v>2003</v>
       </c>
       <c r="E36" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F36" t="str">
-        <f>CONCATENATE($N$2,B36,$N$2,"=",$N$2,E36,"_",D36,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S2001000"="ageyear_2003",</v>
       </c>
     </row>
@@ -5029,14 +6406,14 @@
         <v>308</v>
       </c>
       <c r="D37" t="str">
-        <f>RIGHT(C37,4)</f>
+        <f t="shared" si="2"/>
         <v>2004</v>
       </c>
       <c r="E37" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F37" t="str">
-        <f>CONCATENATE($N$2,B37,$N$2,"=",$N$2,E37,"_",D37,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S3801100"="ageyear_2004",</v>
       </c>
     </row>
@@ -5051,14 +6428,14 @@
         <v>312</v>
       </c>
       <c r="D38" t="str">
-        <f>RIGHT(C38,4)</f>
+        <f t="shared" si="2"/>
         <v>2005</v>
       </c>
       <c r="E38" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F38" t="str">
-        <f>CONCATENATE($N$2,B38,$N$2,"=",$N$2,E38,"_",D38,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S5401000"="ageyear_2005",</v>
       </c>
     </row>
@@ -5073,14 +6450,14 @@
         <v>316</v>
       </c>
       <c r="D39" t="str">
-        <f>RIGHT(C39,4)</f>
+        <f t="shared" si="2"/>
         <v>2006</v>
       </c>
       <c r="E39" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F39" t="str">
-        <f>CONCATENATE($N$2,B39,$N$2,"=",$N$2,E39,"_",D39,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"S7501200"="ageyear_2006",</v>
       </c>
     </row>
@@ -5095,14 +6472,14 @@
         <v>320</v>
       </c>
       <c r="D40" t="str">
-        <f>RIGHT(C40,4)</f>
+        <f t="shared" si="2"/>
         <v>2007</v>
       </c>
       <c r="E40" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F40" t="str">
-        <f>CONCATENATE($N$2,B40,$N$2,"=",$N$2,E40,"_",D40,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T0008500"="ageyear_2007",</v>
       </c>
     </row>
@@ -5117,14 +6494,14 @@
         <v>324</v>
       </c>
       <c r="D41" t="str">
-        <f>RIGHT(C41,4)</f>
+        <f t="shared" si="2"/>
         <v>2008</v>
       </c>
       <c r="E41" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F41" t="str">
-        <f>CONCATENATE($N$2,B41,$N$2,"=",$N$2,E41,"_",D41,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T2011100"="ageyear_2008",</v>
       </c>
     </row>
@@ -5139,14 +6516,14 @@
         <v>328</v>
       </c>
       <c r="D42" t="str">
-        <f>RIGHT(C42,4)</f>
+        <f t="shared" si="2"/>
         <v>2009</v>
       </c>
       <c r="E42" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F42" t="str">
-        <f>CONCATENATE($N$2,B42,$N$2,"=",$N$2,E42,"_",D42,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T3601500"="ageyear_2009",</v>
       </c>
     </row>
@@ -5161,14 +6538,14 @@
         <v>332</v>
       </c>
       <c r="D43" t="str">
-        <f>RIGHT(C43,4)</f>
+        <f t="shared" si="2"/>
         <v>2010</v>
       </c>
       <c r="E43" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F43" t="str">
-        <f>CONCATENATE($N$2,B43,$N$2,"=",$N$2,E43,"_",D43,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T5201400"="ageyear_2010",</v>
       </c>
     </row>
@@ -5183,14 +6560,14 @@
         <v>336</v>
       </c>
       <c r="D44" t="str">
-        <f>RIGHT(C44,4)</f>
+        <f t="shared" si="2"/>
         <v>2011</v>
       </c>
       <c r="E44" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F44" t="str">
-        <f>CONCATENATE($N$2,B44,$N$2,"=",$N$2,E44,"_",D44,$N$2,$O$2)</f>
+        <f t="shared" si="1"/>
         <v>"T6651300"="ageyear_2011",</v>
       </c>
     </row>
@@ -5205,7 +6582,7 @@
         <v>101</v>
       </c>
       <c r="D45" t="str">
-        <f>RIGHT(C45,4)</f>
+        <f t="shared" si="2"/>
         <v>1997</v>
       </c>
       <c r="E45" s="50" t="s">
@@ -5230,14 +6607,14 @@
         <v>78</v>
       </c>
       <c r="D46" t="str">
-        <f>RIGHT(C46,4)</f>
+        <f t="shared" si="2"/>
         <v>2002</v>
       </c>
       <c r="E46" s="50" t="s">
         <v>39</v>
       </c>
       <c r="F46" t="str">
-        <f>CONCATENATE($N$2,B46,$N$2,"=",$N$2,E46,"_",D46,$N$2,$O$2)</f>
+        <f t="shared" ref="F46:F79" si="3">CONCATENATE($N$2,B46,$N$2,"=",$N$2,E46,"_",D46,$N$2,$O$2)</f>
         <v>"S0919700"="todo_2002",</v>
       </c>
     </row>
@@ -5252,14 +6629,14 @@
         <v>152</v>
       </c>
       <c r="D47" t="str">
-        <f>RIGHT(C47,4)</f>
+        <f t="shared" si="2"/>
         <v>2005</v>
       </c>
       <c r="E47" s="50" t="s">
         <v>39</v>
       </c>
       <c r="F47" t="str">
-        <f>CONCATENATE($N$2,B47,$N$2,"=",$N$2,E47,"_",D47,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S6317100"="todo_2005",</v>
       </c>
     </row>
@@ -5274,14 +6651,14 @@
         <v>192</v>
       </c>
       <c r="D48" t="str">
-        <f>RIGHT(C48,4)</f>
+        <f t="shared" si="2"/>
         <v>2008</v>
       </c>
       <c r="E48" s="50" t="s">
         <v>39</v>
       </c>
       <c r="F48" t="str">
-        <f>CONCATENATE($N$2,B48,$N$2,"=",$N$2,E48,"_",D48,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T2782200"="todo_2008",</v>
       </c>
     </row>
@@ -5296,14 +6673,14 @@
         <v>252</v>
       </c>
       <c r="D49" t="str">
-        <f>RIGHT(C49,4)</f>
+        <f t="shared" si="2"/>
         <v>2011</v>
       </c>
       <c r="E49" s="50" t="s">
         <v>39</v>
       </c>
       <c r="F49" t="str">
-        <f>CONCATENATE($N$2,B49,$N$2,"=",$N$2,E49,"_",D49,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T7637800"="todo_2011",</v>
       </c>
     </row>
@@ -5318,14 +6695,14 @@
         <v>71</v>
       </c>
       <c r="D50" t="str">
-        <f>RIGHT(C50,4)</f>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="E50" s="50" t="s">
         <v>59</v>
       </c>
       <c r="F50" t="str">
-        <f>CONCATENATE($N$2,B50,$N$2,"=",$N$2,E50,"_",D50,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"R4893900"="happy_2000",</v>
       </c>
     </row>
@@ -5340,14 +6717,14 @@
         <v>83</v>
       </c>
       <c r="D51" t="str">
-        <f>RIGHT(C51,4)</f>
+        <f t="shared" si="2"/>
         <v>2002</v>
       </c>
       <c r="E51" s="50" t="s">
         <v>59</v>
       </c>
       <c r="F51" t="str">
-        <f>CONCATENATE($N$2,B51,$N$2,"=",$N$2,E51,"_",D51,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S0921100"="happy_2002",</v>
       </c>
     </row>
@@ -5362,14 +6739,14 @@
         <v>92</v>
       </c>
       <c r="D52" t="str">
-        <f>RIGHT(C52,4)</f>
+        <f t="shared" si="2"/>
         <v>2004</v>
       </c>
       <c r="E52" s="50" t="s">
         <v>59</v>
       </c>
       <c r="F52" t="str">
-        <f>CONCATENATE($N$2,B52,$N$2,"=",$N$2,E52,"_",D52,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S4682200"="happy_2004",</v>
       </c>
     </row>
@@ -5384,14 +6761,14 @@
         <v>166</v>
       </c>
       <c r="D53" t="str">
-        <f>RIGHT(C53,4)</f>
+        <f t="shared" si="2"/>
         <v>2006</v>
       </c>
       <c r="E53" s="50" t="s">
         <v>59</v>
       </c>
       <c r="F53" t="str">
-        <f>CONCATENATE($N$2,B53,$N$2,"=",$N$2,E53,"_",D53,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S8332600"="happy_2006",</v>
       </c>
     </row>
@@ -5406,14 +6783,14 @@
         <v>204</v>
       </c>
       <c r="D54" t="str">
-        <f>RIGHT(C54,4)</f>
+        <f t="shared" si="2"/>
         <v>2008</v>
       </c>
       <c r="E54" s="50" t="s">
         <v>59</v>
       </c>
       <c r="F54" t="str">
-        <f>CONCATENATE($N$2,B54,$N$2,"=",$N$2,E54,"_",D54,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T2782900"="happy_2008",</v>
       </c>
     </row>
@@ -5428,14 +6805,14 @@
         <v>230</v>
       </c>
       <c r="D55" t="str">
-        <f>RIGHT(C55,4)</f>
+        <f t="shared" si="2"/>
         <v>2010</v>
       </c>
       <c r="E55" s="50" t="s">
         <v>59</v>
       </c>
       <c r="F55" t="str">
-        <f>CONCATENATE($N$2,B55,$N$2,"=",$N$2,E55,"_",D55,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T6144000"="happy_2010",</v>
       </c>
     </row>
@@ -5450,14 +6827,14 @@
         <v>68</v>
       </c>
       <c r="D56" t="str">
-        <f>RIGHT(C56,4)</f>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="E56" s="50" t="s">
         <v>61</v>
       </c>
       <c r="F56" t="str">
-        <f>CONCATENATE($N$2,B56,$N$2,"=",$N$2,E56,"_",D56,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"R4893600"="nervous_2000",</v>
       </c>
     </row>
@@ -5472,14 +6849,14 @@
         <v>80</v>
       </c>
       <c r="D57" t="str">
-        <f>RIGHT(C57,4)</f>
+        <f t="shared" si="2"/>
         <v>2002</v>
       </c>
       <c r="E57" s="50" t="s">
         <v>61</v>
       </c>
       <c r="F57" t="str">
-        <f>CONCATENATE($N$2,B57,$N$2,"=",$N$2,E57,"_",D57,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S0920800"="nervous_2002",</v>
       </c>
     </row>
@@ -5494,14 +6871,14 @@
         <v>89</v>
       </c>
       <c r="D58" t="str">
-        <f>RIGHT(C58,4)</f>
+        <f t="shared" si="2"/>
         <v>2004</v>
       </c>
       <c r="E58" s="50" t="s">
         <v>61</v>
       </c>
       <c r="F58" t="str">
-        <f>CONCATENATE($N$2,B58,$N$2,"=",$N$2,E58,"_",D58,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S4681900"="nervous_2004",</v>
       </c>
     </row>
@@ -5516,14 +6893,14 @@
         <v>160</v>
       </c>
       <c r="D59" t="str">
-        <f>RIGHT(C59,4)</f>
+        <f t="shared" si="2"/>
         <v>2006</v>
       </c>
       <c r="E59" s="50" t="s">
         <v>61</v>
       </c>
       <c r="F59" t="str">
-        <f>CONCATENATE($N$2,B59,$N$2,"=",$N$2,E59,"_",D59,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S8332300"="nervous_2006",</v>
       </c>
     </row>
@@ -5538,14 +6915,14 @@
         <v>198</v>
       </c>
       <c r="D60" t="str">
-        <f>RIGHT(C60,4)</f>
+        <f t="shared" si="2"/>
         <v>2008</v>
       </c>
       <c r="E60" s="50" t="s">
         <v>61</v>
       </c>
       <c r="F60" t="str">
-        <f>CONCATENATE($N$2,B60,$N$2,"=",$N$2,E60,"_",D60,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T2782600"="nervous_2008",</v>
       </c>
     </row>
@@ -5560,14 +6937,14 @@
         <v>224</v>
       </c>
       <c r="D61" t="str">
-        <f>RIGHT(C61,4)</f>
+        <f t="shared" si="2"/>
         <v>2010</v>
       </c>
       <c r="E61" s="50" t="s">
         <v>61</v>
       </c>
       <c r="F61" t="str">
-        <f>CONCATENATE($N$2,B61,$N$2,"=",$N$2,E61,"_",D61,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T6143700"="nervous_2010",</v>
       </c>
     </row>
@@ -5582,14 +6959,14 @@
         <v>69</v>
       </c>
       <c r="D62" t="str">
-        <f>RIGHT(C62,4)</f>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="E62" s="50" t="s">
         <v>340</v>
       </c>
       <c r="F62" t="str">
-        <f>CONCATENATE($N$2,B62,$N$2,"=",$N$2,E62,"_",D62,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"R4893700"="calm_2000",</v>
       </c>
     </row>
@@ -5604,14 +6981,14 @@
         <v>81</v>
       </c>
       <c r="D63" t="str">
-        <f>RIGHT(C63,4)</f>
+        <f t="shared" si="2"/>
         <v>2002</v>
       </c>
       <c r="E63" s="50" t="s">
         <v>340</v>
       </c>
       <c r="F63" t="str">
-        <f>CONCATENATE($N$2,B63,$N$2,"=",$N$2,E63,"_",D63,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S0920900"="calm_2002",</v>
       </c>
     </row>
@@ -5626,14 +7003,14 @@
         <v>90</v>
       </c>
       <c r="D64" t="str">
-        <f>RIGHT(C64,4)</f>
+        <f t="shared" si="2"/>
         <v>2004</v>
       </c>
       <c r="E64" s="50" t="s">
         <v>340</v>
       </c>
       <c r="F64" t="str">
-        <f>CONCATENATE($N$2,B64,$N$2,"=",$N$2,E64,"_",D64,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S4682000"="calm_2004",</v>
       </c>
     </row>
@@ -5648,14 +7025,14 @@
         <v>162</v>
       </c>
       <c r="D65" t="str">
-        <f>RIGHT(C65,4)</f>
+        <f t="shared" si="2"/>
         <v>2006</v>
       </c>
       <c r="E65" s="50" t="s">
         <v>340</v>
       </c>
       <c r="F65" t="str">
-        <f>CONCATENATE($N$2,B65,$N$2,"=",$N$2,E65,"_",D65,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S8332400"="calm_2006",</v>
       </c>
     </row>
@@ -5670,14 +7047,14 @@
         <v>200</v>
       </c>
       <c r="D66" t="str">
-        <f>RIGHT(C66,4)</f>
+        <f t="shared" ref="D66:D97" si="4">RIGHT(C66,4)</f>
         <v>2008</v>
       </c>
       <c r="E66" s="50" t="s">
         <v>340</v>
       </c>
       <c r="F66" t="str">
-        <f>CONCATENATE($N$2,B66,$N$2,"=",$N$2,E66,"_",D66,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T2782700"="calm_2008",</v>
       </c>
     </row>
@@ -5692,14 +7069,14 @@
         <v>226</v>
       </c>
       <c r="D67" t="str">
-        <f>RIGHT(C67,4)</f>
+        <f t="shared" si="4"/>
         <v>2010</v>
       </c>
       <c r="E67" s="50" t="s">
         <v>340</v>
       </c>
       <c r="F67" t="str">
-        <f>CONCATENATE($N$2,B67,$N$2,"=",$N$2,E67,"_",D67,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T6143800"="calm_2010",</v>
       </c>
     </row>
@@ -5714,14 +7091,14 @@
         <v>72</v>
       </c>
       <c r="D68" t="str">
-        <f>RIGHT(C68,4)</f>
+        <f t="shared" si="4"/>
         <v>2000</v>
       </c>
       <c r="E68" s="50" t="s">
         <v>60</v>
       </c>
       <c r="F68" t="str">
-        <f>CONCATENATE($N$2,B68,$N$2,"=",$N$2,E68,"_",D68,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"R4894000"="depressed_2000",</v>
       </c>
     </row>
@@ -5736,14 +7113,14 @@
         <v>84</v>
       </c>
       <c r="D69" t="str">
-        <f>RIGHT(C69,4)</f>
+        <f t="shared" si="4"/>
         <v>2002</v>
       </c>
       <c r="E69" s="50" t="s">
         <v>60</v>
       </c>
       <c r="F69" t="str">
-        <f>CONCATENATE($N$2,B69,$N$2,"=",$N$2,E69,"_",D69,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S0921200"="depressed_2002",</v>
       </c>
     </row>
@@ -5758,14 +7135,14 @@
         <v>138</v>
       </c>
       <c r="D70" t="str">
-        <f>RIGHT(C70,4)</f>
+        <f t="shared" si="4"/>
         <v>2004</v>
       </c>
       <c r="E70" s="50" t="s">
         <v>60</v>
       </c>
       <c r="F70" t="str">
-        <f>CONCATENATE($N$2,B70,$N$2,"=",$N$2,E70,"_",D70,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S4682300"="depressed_2004",</v>
       </c>
     </row>
@@ -5780,14 +7157,14 @@
         <v>168</v>
       </c>
       <c r="D71" t="str">
-        <f>RIGHT(C71,4)</f>
+        <f t="shared" si="4"/>
         <v>2006</v>
       </c>
       <c r="E71" s="50" t="s">
         <v>60</v>
       </c>
       <c r="F71" t="str">
-        <f>CONCATENATE($N$2,B71,$N$2,"=",$N$2,E71,"_",D71,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S8332700"="depressed_2006",</v>
       </c>
     </row>
@@ -5802,14 +7179,14 @@
         <v>206</v>
       </c>
       <c r="D72" t="str">
-        <f>RIGHT(C72,4)</f>
+        <f t="shared" si="4"/>
         <v>2008</v>
       </c>
       <c r="E72" s="50" t="s">
         <v>60</v>
       </c>
       <c r="F72" t="str">
-        <f>CONCATENATE($N$2,B72,$N$2,"=",$N$2,E72,"_",D72,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T2783000"="depressed_2008",</v>
       </c>
     </row>
@@ -5824,14 +7201,14 @@
         <v>232</v>
       </c>
       <c r="D73" t="str">
-        <f>RIGHT(C73,4)</f>
+        <f t="shared" si="4"/>
         <v>2010</v>
       </c>
       <c r="E73" s="50" t="s">
         <v>60</v>
       </c>
       <c r="F73" t="str">
-        <f>CONCATENATE($N$2,B73,$N$2,"=",$N$2,E73,"_",D73,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T6144100"="depressed_2010",</v>
       </c>
     </row>
@@ -5846,14 +7223,14 @@
         <v>70</v>
       </c>
       <c r="D74" t="str">
-        <f>RIGHT(C74,4)</f>
+        <f t="shared" si="4"/>
         <v>2000</v>
       </c>
       <c r="E74" s="50" t="s">
         <v>58</v>
       </c>
       <c r="F74" t="str">
-        <f>CONCATENATE($N$2,B74,$N$2,"=",$N$2,E74,"_",D74,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"R4893800"="blue_2000",</v>
       </c>
     </row>
@@ -5868,14 +7245,14 @@
         <v>82</v>
       </c>
       <c r="D75" t="str">
-        <f>RIGHT(C75,4)</f>
+        <f t="shared" si="4"/>
         <v>2002</v>
       </c>
       <c r="E75" s="50" t="s">
         <v>58</v>
       </c>
       <c r="F75" t="str">
-        <f>CONCATENATE($N$2,B75,$N$2,"=",$N$2,E75,"_",D75,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S0921000"="blue_2002",</v>
       </c>
     </row>
@@ -5890,14 +7267,14 @@
         <v>91</v>
       </c>
       <c r="D76" t="str">
-        <f>RIGHT(C76,4)</f>
+        <f t="shared" si="4"/>
         <v>2004</v>
       </c>
       <c r="E76" s="50" t="s">
         <v>58</v>
       </c>
       <c r="F76" t="str">
-        <f>CONCATENATE($N$2,B76,$N$2,"=",$N$2,E76,"_",D76,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S4682100"="blue_2004",</v>
       </c>
     </row>
@@ -5912,14 +7289,14 @@
         <v>164</v>
       </c>
       <c r="D77" t="str">
-        <f>RIGHT(C77,4)</f>
+        <f t="shared" si="4"/>
         <v>2006</v>
       </c>
       <c r="E77" s="50" t="s">
         <v>58</v>
       </c>
       <c r="F77" t="str">
-        <f>CONCATENATE($N$2,B77,$N$2,"=",$N$2,E77,"_",D77,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"S8332500"="blue_2006",</v>
       </c>
     </row>
@@ -5934,14 +7311,14 @@
         <v>202</v>
       </c>
       <c r="D78" t="str">
-        <f>RIGHT(C78,4)</f>
+        <f t="shared" si="4"/>
         <v>2008</v>
       </c>
       <c r="E78" s="50" t="s">
         <v>58</v>
       </c>
       <c r="F78" t="str">
-        <f>CONCATENATE($N$2,B78,$N$2,"=",$N$2,E78,"_",D78,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T2782800"="blue_2008",</v>
       </c>
     </row>
@@ -5956,14 +7333,14 @@
         <v>228</v>
       </c>
       <c r="D79" t="str">
-        <f>RIGHT(C79,4)</f>
+        <f t="shared" si="4"/>
         <v>2010</v>
       </c>
       <c r="E79" s="50" t="s">
         <v>58</v>
       </c>
       <c r="F79" t="str">
-        <f>CONCATENATE($N$2,B79,$N$2,"=",$N$2,E79,"_",D79,$N$2,$O$2)</f>
+        <f t="shared" si="3"/>
         <v>"T6143900"="blue_2010",</v>
       </c>
     </row>
@@ -5978,7 +7355,7 @@
         <v>276</v>
       </c>
       <c r="D80" t="str">
-        <f>RIGHT(C80,4)</f>
+        <f t="shared" si="4"/>
         <v>1997</v>
       </c>
       <c r="E80" s="50" t="s">
@@ -6003,14 +7380,14 @@
         <v>67</v>
       </c>
       <c r="D81" t="str">
-        <f>RIGHT(C81,4)</f>
+        <f t="shared" si="4"/>
         <v>2000</v>
       </c>
       <c r="E81" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F81" t="str">
-        <f>CONCATENATE($N$2,B81,$N$2,"=",$N$2,E81,"_",D81,$N$2,$O$2)</f>
+        <f t="shared" ref="F81:F103" si="5">CONCATENATE($N$2,B81,$N$2,"=",$N$2,E81,"_",D81,$N$2,$O$2)</f>
         <v>"R4893400"="attend_2000",</v>
       </c>
     </row>
@@ -6025,14 +7402,14 @@
         <v>73</v>
       </c>
       <c r="D82" t="str">
-        <f>RIGHT(C82,4)</f>
+        <f t="shared" si="4"/>
         <v>2001</v>
       </c>
       <c r="E82" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F82" t="str">
-        <f>CONCATENATE($N$2,B82,$N$2,"=",$N$2,E82,"_",D82,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"R6520100"="attend_2001",</v>
       </c>
     </row>
@@ -6047,14 +7424,14 @@
         <v>74</v>
       </c>
       <c r="D83" t="str">
-        <f>RIGHT(C83,4)</f>
+        <f t="shared" si="4"/>
         <v>2002</v>
       </c>
       <c r="E83" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F83" t="str">
-        <f>CONCATENATE($N$2,B83,$N$2,"=",$N$2,E83,"_",D83,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"S0919300"="attend_2002",</v>
       </c>
     </row>
@@ -6069,14 +7446,14 @@
         <v>87</v>
       </c>
       <c r="D84" t="str">
-        <f>RIGHT(C84,4)</f>
+        <f t="shared" si="4"/>
         <v>2003</v>
       </c>
       <c r="E84" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F84" t="str">
-        <f>CONCATENATE($N$2,B84,$N$2,"=",$N$2,E84,"_",D84,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"S2987800"="attend_2003",</v>
       </c>
     </row>
@@ -6091,14 +7468,14 @@
         <v>88</v>
       </c>
       <c r="D85" t="str">
-        <f>RIGHT(C85,4)</f>
+        <f t="shared" si="4"/>
         <v>2004</v>
       </c>
       <c r="E85" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F85" t="str">
-        <f>CONCATENATE($N$2,B85,$N$2,"=",$N$2,E85,"_",D85,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"S4681700"="attend_2004",</v>
       </c>
     </row>
@@ -6113,14 +7490,14 @@
         <v>144</v>
       </c>
       <c r="D86" t="str">
-        <f>RIGHT(C86,4)</f>
+        <f t="shared" si="4"/>
         <v>2005</v>
       </c>
       <c r="E86" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F86" t="str">
-        <f>CONCATENATE($N$2,B86,$N$2,"=",$N$2,E86,"_",D86,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"S6316700"="attend_2005",</v>
       </c>
     </row>
@@ -6135,14 +7512,14 @@
         <v>158</v>
       </c>
       <c r="D87" t="str">
-        <f>RIGHT(C87,4)</f>
+        <f t="shared" si="4"/>
         <v>2006</v>
       </c>
       <c r="E87" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F87" t="str">
-        <f>CONCATENATE($N$2,B87,$N$2,"=",$N$2,E87,"_",D87,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"S8331500"="attend_2006",</v>
       </c>
     </row>
@@ -6157,14 +7534,14 @@
         <v>172</v>
       </c>
       <c r="D88" t="str">
-        <f>RIGHT(C88,4)</f>
+        <f t="shared" si="4"/>
         <v>2007</v>
       </c>
       <c r="E88" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F88" t="str">
-        <f>CONCATENATE($N$2,B88,$N$2,"=",$N$2,E88,"_",D88,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T0739400"="attend_2007",</v>
       </c>
     </row>
@@ -6179,14 +7556,14 @@
         <v>184</v>
       </c>
       <c r="D89" t="str">
-        <f>RIGHT(C89,4)</f>
+        <f t="shared" si="4"/>
         <v>2008</v>
       </c>
       <c r="E89" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F89" t="str">
-        <f>CONCATENATE($N$2,B89,$N$2,"=",$N$2,E89,"_",D89,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T2781700"="attend_2008",</v>
       </c>
     </row>
@@ -6201,14 +7578,14 @@
         <v>214</v>
       </c>
       <c r="D90" t="str">
-        <f>RIGHT(C90,4)</f>
+        <f t="shared" si="4"/>
         <v>2009</v>
       </c>
       <c r="E90" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F90" t="str">
-        <f>CONCATENATE($N$2,B90,$N$2,"=",$N$2,E90,"_",D90,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T4495000"="attend_2009",</v>
       </c>
     </row>
@@ -6223,14 +7600,14 @@
         <v>222</v>
       </c>
       <c r="D91" t="str">
-        <f>RIGHT(C91,4)</f>
+        <f t="shared" si="4"/>
         <v>2010</v>
       </c>
       <c r="E91" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F91" t="str">
-        <f>CONCATENATE($N$2,B91,$N$2,"=",$N$2,E91,"_",D91,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T6143400"="attend_2010",</v>
       </c>
     </row>
@@ -6245,14 +7622,14 @@
         <v>244</v>
       </c>
       <c r="D92" t="str">
-        <f>RIGHT(C92,4)</f>
+        <f t="shared" si="4"/>
         <v>2011</v>
       </c>
       <c r="E92" s="50" t="s">
         <v>26</v>
       </c>
       <c r="F92" t="str">
-        <f>CONCATENATE($N$2,B92,$N$2,"=",$N$2,E92,"_",D92,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T7637300"="attend_2011",</v>
       </c>
     </row>
@@ -6267,14 +7644,14 @@
         <v>85</v>
       </c>
       <c r="D93" t="str">
-        <f>RIGHT(C93,4)</f>
+        <f t="shared" si="4"/>
         <v>2002</v>
       </c>
       <c r="E93" s="50" t="s">
         <v>50</v>
       </c>
       <c r="F93" t="str">
-        <f>CONCATENATE($N$2,B93,$N$2,"=",$N$2,E93,"_",D93,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"S1225400"="computer_2002",</v>
       </c>
     </row>
@@ -6289,14 +7666,14 @@
         <v>174</v>
       </c>
       <c r="D94" t="str">
-        <f>RIGHT(C94,4)</f>
+        <f t="shared" si="4"/>
         <v>2007</v>
       </c>
       <c r="E94" s="50" t="s">
         <v>50</v>
       </c>
       <c r="F94" t="str">
-        <f>CONCATENATE($N$2,B94,$N$2,"=",$N$2,E94,"_",D94,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T1049900"="computer_2007",</v>
       </c>
     </row>
@@ -6311,14 +7688,14 @@
         <v>208</v>
       </c>
       <c r="D95" t="str">
-        <f>RIGHT(C95,4)</f>
+        <f t="shared" si="4"/>
         <v>2008</v>
       </c>
       <c r="E95" s="50" t="s">
         <v>50</v>
       </c>
       <c r="F95" t="str">
-        <f>CONCATENATE($N$2,B95,$N$2,"=",$N$2,E95,"_",D95,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T3145100"="computer_2008",</v>
       </c>
     </row>
@@ -6333,14 +7710,14 @@
         <v>216</v>
       </c>
       <c r="D96" t="str">
-        <f>RIGHT(C96,4)</f>
+        <f t="shared" si="4"/>
         <v>2009</v>
       </c>
       <c r="E96" s="50" t="s">
         <v>50</v>
       </c>
       <c r="F96" t="str">
-        <f>CONCATENATE($N$2,B96,$N$2,"=",$N$2,E96,"_",D96,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T4565400"="computer_2009",</v>
       </c>
     </row>
@@ -6355,14 +7732,14 @@
         <v>234</v>
       </c>
       <c r="D97" t="str">
-        <f>RIGHT(C97,4)</f>
+        <f t="shared" si="4"/>
         <v>2010</v>
       </c>
       <c r="E97" s="50" t="s">
         <v>50</v>
       </c>
       <c r="F97" t="str">
-        <f>CONCATENATE($N$2,B97,$N$2,"=",$N$2,E97,"_",D97,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T6209600"="computer_2010",</v>
       </c>
     </row>
@@ -6377,14 +7754,14 @@
         <v>258</v>
       </c>
       <c r="D98" t="str">
-        <f>RIGHT(C98,4)</f>
+        <f t="shared" ref="D98:D129" si="6">RIGHT(C98,4)</f>
         <v>2011</v>
       </c>
       <c r="E98" s="50" t="s">
         <v>50</v>
       </c>
       <c r="F98" t="str">
-        <f>CONCATENATE($N$2,B98,$N$2,"=",$N$2,E98,"_",D98,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T7707000"="computer_2011",</v>
       </c>
     </row>
@@ -6399,14 +7776,14 @@
         <v>86</v>
       </c>
       <c r="D99" t="str">
-        <f>RIGHT(C99,4)</f>
+        <f t="shared" si="6"/>
         <v>2002</v>
       </c>
       <c r="E99" s="50" t="s">
         <v>52</v>
       </c>
       <c r="F99" t="str">
-        <f>CONCATENATE($N$2,B99,$N$2,"=",$N$2,E99,"_",D99,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"S1225500"="tv_2002",</v>
       </c>
     </row>
@@ -6421,14 +7798,14 @@
         <v>176</v>
       </c>
       <c r="D100" t="str">
-        <f>RIGHT(C100,4)</f>
+        <f t="shared" si="6"/>
         <v>2007</v>
       </c>
       <c r="E100" s="50" t="s">
         <v>52</v>
       </c>
       <c r="F100" t="str">
-        <f>CONCATENATE($N$2,B100,$N$2,"=",$N$2,E100,"_",D100,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T1050000"="tv_2007",</v>
       </c>
     </row>
@@ -6443,14 +7820,14 @@
         <v>210</v>
       </c>
       <c r="D101" t="str">
-        <f>RIGHT(C101,4)</f>
+        <f t="shared" si="6"/>
         <v>2008</v>
       </c>
       <c r="E101" s="50" t="s">
         <v>52</v>
       </c>
       <c r="F101" t="str">
-        <f>CONCATENATE($N$2,B101,$N$2,"=",$N$2,E101,"_",D101,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T3145200"="tv_2008",</v>
       </c>
     </row>
@@ -6465,14 +7842,14 @@
         <v>218</v>
       </c>
       <c r="D102" t="str">
-        <f>RIGHT(C102,4)</f>
+        <f t="shared" si="6"/>
         <v>2009</v>
       </c>
       <c r="E102" s="50" t="s">
         <v>52</v>
       </c>
       <c r="F102" t="str">
-        <f>CONCATENATE($N$2,B102,$N$2,"=",$N$2,E102,"_",D102,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T4565500"="tv_2009",</v>
       </c>
     </row>
@@ -6487,14 +7864,14 @@
         <v>236</v>
       </c>
       <c r="D103" t="str">
-        <f>RIGHT(C103,4)</f>
+        <f t="shared" si="6"/>
         <v>2010</v>
       </c>
       <c r="E103" s="50" t="s">
         <v>52</v>
       </c>
       <c r="F103" t="str">
-        <f>CONCATENATE($N$2,B103,$N$2,"=",$N$2,E103,"_",D103,$N$2,$O$2)</f>
+        <f t="shared" si="5"/>
         <v>"T6209700"="tv_2010",</v>
       </c>
     </row>
@@ -6509,7 +7886,7 @@
         <v>260</v>
       </c>
       <c r="D104" t="str">
-        <f>RIGHT(C104,4)</f>
+        <f t="shared" si="6"/>
         <v>2011</v>
       </c>
       <c r="E104" s="50" t="s">
@@ -6531,7 +7908,7 @@
         <v>196</v>
       </c>
       <c r="D105" t="str">
-        <f>RIGHT(C105,4)</f>
+        <f t="shared" si="6"/>
         <v>2008</v>
       </c>
       <c r="E105" s="50" t="s">
@@ -6553,7 +7930,7 @@
         <v>256</v>
       </c>
       <c r="D106" t="str">
-        <f>RIGHT(C106,4)</f>
+        <f t="shared" si="6"/>
         <v>2011</v>
       </c>
       <c r="E106" s="50" t="s">
@@ -6578,7 +7955,7 @@
         <v>98</v>
       </c>
       <c r="D107" t="str">
-        <f>RIGHT(C107,4)</f>
+        <f t="shared" si="6"/>
         <v>1997</v>
       </c>
       <c r="E107" s="50" t="s">
@@ -6603,14 +7980,14 @@
         <v>98</v>
       </c>
       <c r="D108" t="str">
-        <f>RIGHT(C108,4)</f>
+        <f t="shared" si="6"/>
         <v>1997</v>
       </c>
       <c r="E108" s="50" t="s">
         <v>15</v>
       </c>
       <c r="F108" t="str">
-        <f t="shared" ref="F108:F111" si="0">CONCATENATE($N$2,B108,$N$2,"=",$N$2,E108,$N$2,$O$2)</f>
+        <f t="shared" ref="F108:F111" si="7">CONCATENATE($N$2,B108,$N$2,"=",$N$2,E108,$N$2,$O$2)</f>
         <v>"R0536402"="byear",</v>
       </c>
       <c r="G108" t="s">
@@ -6628,14 +8005,14 @@
         <v>103</v>
       </c>
       <c r="D109" t="str">
-        <f>RIGHT(C109,4)</f>
+        <f t="shared" si="6"/>
         <v>1997</v>
       </c>
       <c r="E109" s="50" t="s">
         <v>16</v>
       </c>
       <c r="F109" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>"R1482600"="race",</v>
       </c>
       <c r="G109" t="s">
@@ -6653,14 +8030,14 @@
         <v>96</v>
       </c>
       <c r="D110" t="str">
-        <f>RIGHT(C110,4)</f>
+        <f t="shared" si="6"/>
         <v>1997</v>
       </c>
       <c r="E110" s="50" t="s">
         <v>17</v>
       </c>
       <c r="F110" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>"R0536300"="sex",</v>
       </c>
       <c r="G110" t="s">
@@ -6678,14 +8055,14 @@
         <v>62</v>
       </c>
       <c r="D111" t="str">
-        <f>RIGHT(C111,4)</f>
+        <f t="shared" si="6"/>
         <v>1997</v>
       </c>
       <c r="E111" s="50" t="s">
         <v>18</v>
       </c>
       <c r="F111" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>"R0000100"="id",</v>
       </c>
       <c r="G111" t="s">
@@ -6703,7 +8080,7 @@
         <v>180</v>
       </c>
       <c r="D112" t="str">
-        <f>RIGHT(C112,4)</f>
+        <f t="shared" si="6"/>
         <v>2008</v>
       </c>
       <c r="E112" s="50" t="s">
@@ -6725,14 +8102,14 @@
         <v>240</v>
       </c>
       <c r="D113" t="str">
-        <f>RIGHT(C113,4)</f>
+        <f t="shared" si="6"/>
         <v>2011</v>
       </c>
       <c r="E113" s="50" t="s">
         <v>43</v>
       </c>
       <c r="F113" t="str">
-        <f t="shared" ref="F113:F134" si="1">CONCATENATE($N$2,B113,$N$2,"=",$N$2,E113,"_",D113,$N$2,$O$2)</f>
+        <f t="shared" ref="F113:F132" si="8">CONCATENATE($N$2,B113,$N$2,"=",$N$2,E113,"_",D113,$N$2,$O$2)</f>
         <v>"T6759400"="bornagain_2011",</v>
       </c>
     </row>
@@ -6747,14 +8124,14 @@
         <v>77</v>
       </c>
       <c r="D114" t="str">
-        <f>RIGHT(C114,4)</f>
+        <f t="shared" si="6"/>
         <v>2002</v>
       </c>
       <c r="E114" s="50" t="s">
         <v>37</v>
       </c>
       <c r="F114" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"S0919600"="decisions_2002",</v>
       </c>
     </row>
@@ -6769,14 +8146,14 @@
         <v>150</v>
       </c>
       <c r="D115" t="str">
-        <f>RIGHT(C115,4)</f>
+        <f t="shared" si="6"/>
         <v>2005</v>
       </c>
       <c r="E115" s="50" t="s">
         <v>37</v>
       </c>
       <c r="F115" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"S6317000"="decisions_2005",</v>
       </c>
     </row>
@@ -6791,14 +8168,14 @@
         <v>190</v>
       </c>
       <c r="D116" t="str">
-        <f>RIGHT(C116,4)</f>
+        <f t="shared" si="6"/>
         <v>2008</v>
       </c>
       <c r="E116" s="50" t="s">
         <v>37</v>
       </c>
       <c r="F116" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"T2782100"="decisions_2008",</v>
       </c>
     </row>
@@ -6813,14 +8190,14 @@
         <v>250</v>
       </c>
       <c r="D117" t="str">
-        <f>RIGHT(C117,4)</f>
+        <f t="shared" si="6"/>
         <v>2011</v>
       </c>
       <c r="E117" s="50" t="s">
         <v>37</v>
       </c>
       <c r="F117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"T7637700"="decisions_2011",</v>
       </c>
     </row>
@@ -6835,14 +8212,14 @@
         <v>76</v>
       </c>
       <c r="D118" t="str">
-        <f>RIGHT(C118,4)</f>
+        <f t="shared" si="6"/>
         <v>2002</v>
       </c>
       <c r="E118" s="50" t="s">
         <v>36</v>
       </c>
       <c r="F118" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"S0919500"="obeyed_2002",</v>
       </c>
     </row>
@@ -6857,14 +8234,14 @@
         <v>148</v>
       </c>
       <c r="D119" t="str">
-        <f>RIGHT(C119,4)</f>
+        <f t="shared" si="6"/>
         <v>2005</v>
       </c>
       <c r="E119" s="50" t="s">
         <v>36</v>
       </c>
       <c r="F119" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"S6316900"="obeyed_2005",</v>
       </c>
     </row>
@@ -6879,14 +8256,14 @@
         <v>188</v>
       </c>
       <c r="D120" t="str">
-        <f>RIGHT(C120,4)</f>
+        <f t="shared" si="6"/>
         <v>2008</v>
       </c>
       <c r="E120" s="50" t="s">
         <v>36</v>
       </c>
       <c r="F120" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"T2782000"="obeyed_2008",</v>
       </c>
     </row>
@@ -6901,14 +8278,14 @@
         <v>248</v>
       </c>
       <c r="D121" t="str">
-        <f>RIGHT(C121,4)</f>
+        <f t="shared" si="6"/>
         <v>2011</v>
       </c>
       <c r="E121" s="50" t="s">
         <v>36</v>
       </c>
       <c r="F121" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"T7637600"="obeyed_2011",</v>
       </c>
     </row>
@@ -6923,14 +8300,14 @@
         <v>140</v>
       </c>
       <c r="D122" t="str">
-        <f>RIGHT(C122,4)</f>
+        <f t="shared" si="6"/>
         <v>2005</v>
       </c>
       <c r="E122" s="50" t="s">
         <v>48</v>
       </c>
       <c r="F122" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"S5532800"="relpref_2005",</v>
       </c>
     </row>
@@ -6945,14 +8322,14 @@
         <v>178</v>
       </c>
       <c r="D123" t="str">
-        <f>RIGHT(C123,4)</f>
+        <f t="shared" si="6"/>
         <v>2008</v>
       </c>
       <c r="E123" s="50" t="s">
         <v>48</v>
       </c>
       <c r="F123" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"T2111400"="relpref_2008",</v>
       </c>
     </row>
@@ -6967,14 +8344,14 @@
         <v>238</v>
       </c>
       <c r="D124" t="str">
-        <f>RIGHT(C124,4)</f>
+        <f t="shared" si="6"/>
         <v>2011</v>
       </c>
       <c r="E124" s="50" t="s">
         <v>48</v>
       </c>
       <c r="F124" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"T6759300"="relpref_2011",</v>
       </c>
     </row>
@@ -6989,14 +8366,14 @@
         <v>75</v>
       </c>
       <c r="D125" t="str">
-        <f>RIGHT(C125,4)</f>
+        <f t="shared" si="6"/>
         <v>2002</v>
       </c>
       <c r="E125" s="50" t="s">
         <v>35</v>
       </c>
       <c r="F125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"S0919400"="values_2002",</v>
       </c>
     </row>
@@ -7011,14 +8388,14 @@
         <v>146</v>
       </c>
       <c r="D126" t="str">
-        <f>RIGHT(C126,4)</f>
+        <f t="shared" si="6"/>
         <v>2005</v>
       </c>
       <c r="E126" s="50" t="s">
         <v>35</v>
       </c>
       <c r="F126" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"S6316800"="values_2005",</v>
       </c>
     </row>
@@ -7033,14 +8410,14 @@
         <v>186</v>
       </c>
       <c r="D127" t="str">
-        <f>RIGHT(C127,4)</f>
+        <f t="shared" si="6"/>
         <v>2008</v>
       </c>
       <c r="E127" s="50" t="s">
         <v>35</v>
       </c>
       <c r="F127" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"T2781900"="values_2008",</v>
       </c>
     </row>
@@ -7055,14 +8432,14 @@
         <v>246</v>
       </c>
       <c r="D128" t="str">
-        <f>RIGHT(C128,4)</f>
+        <f t="shared" si="6"/>
         <v>2011</v>
       </c>
       <c r="E128" s="50" t="s">
         <v>35</v>
       </c>
       <c r="F128" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"T7637500"="values_2011",</v>
       </c>
     </row>
@@ -7077,14 +8454,14 @@
         <v>79</v>
       </c>
       <c r="D129" t="str">
-        <f>RIGHT(C129,4)</f>
+        <f t="shared" si="6"/>
         <v>2002</v>
       </c>
       <c r="E129" s="50" t="s">
         <v>41</v>
       </c>
       <c r="F129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"S0919800"="pray_2002",</v>
       </c>
     </row>
@@ -7099,14 +8476,14 @@
         <v>154</v>
       </c>
       <c r="D130" t="str">
-        <f>RIGHT(C130,4)</f>
+        <f t="shared" ref="D130:D161" si="9">RIGHT(C130,4)</f>
         <v>2005</v>
       </c>
       <c r="E130" s="50" t="s">
         <v>41</v>
       </c>
       <c r="F130" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"S6317200"="pray_2005",</v>
       </c>
     </row>
@@ -7121,14 +8498,14 @@
         <v>194</v>
       </c>
       <c r="D131" t="str">
-        <f>RIGHT(C131,4)</f>
+        <f t="shared" si="9"/>
         <v>2008</v>
       </c>
       <c r="E131" s="50" t="s">
         <v>41</v>
       </c>
       <c r="F131" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"T2782300"="pray_2008",</v>
       </c>
     </row>
@@ -7143,14 +8520,14 @@
         <v>254</v>
       </c>
       <c r="D132" t="str">
-        <f t="shared" ref="D132:D134" si="2">RIGHT(C132,4)</f>
+        <f t="shared" ref="D132:D134" si="10">RIGHT(C132,4)</f>
         <v>2011</v>
       </c>
       <c r="E132" s="50" t="s">
         <v>41</v>
       </c>
       <c r="F132" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>"T7637900"="pray_2011",</v>
       </c>
     </row>
@@ -7165,14 +8542,14 @@
         <v>344</v>
       </c>
       <c r="D133" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1997</v>
       </c>
       <c r="E133" s="50" t="s">
         <v>342</v>
       </c>
       <c r="F133" t="str">
-        <f t="shared" ref="F133:F134" si="3">CONCATENATE($N$2,B133,$N$2,"=",$N$2,E133,$N$2,$O$2)</f>
+        <f t="shared" ref="F133:F134" si="11">CONCATENATE($N$2,B133,$N$2,"=",$N$2,E133,$N$2,$O$2)</f>
         <v>"R0552300"="relprefPR",</v>
       </c>
       <c r="G133" t="s">
@@ -7190,14 +8567,14 @@
         <v>274</v>
       </c>
       <c r="D134" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1997</v>
       </c>
       <c r="E134" s="50" t="s">
         <v>55</v>
       </c>
       <c r="F134" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>"R0552200"="relraisedPR",</v>
       </c>
       <c r="G134" t="s">
@@ -7225,4 +8602,27 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>